<commit_message>
add in gnu library
</commit_message>
<xml_diff>
--- a/projects/patch_empty_app_partition_2/src/shasta_pmbus.xlsx
+++ b/projects/patch_empty_app_partition_2/src/shasta_pmbus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seetweireniv\Documents\Digital_Workspace\Shasta_TM\shasta_projects\projects\patch_empty_app_partition_2\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seetweireniv\Documents\Digital_Workspace\Shasta_CUS\shasta_projects\projects\patch_empty_app_partition_2\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F007FD8-0EEE-4EC4-8DBD-68A58A0C087D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A25871C-AAA8-49F4-84A0-9EAB83F08D19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shasta" sheetId="8" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13830" uniqueCount="1090">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13828" uniqueCount="1090">
   <si>
     <t>Opcode</t>
   </si>
@@ -6323,7 +6323,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C175" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A179" sqref="A179:U179"/>
+      <selection pane="bottomRight" activeCell="E190" sqref="E190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -40776,7 +40776,7 @@
         <v>99</v>
       </c>
       <c r="E179" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F179" s="9" t="s">
         <v>65</v>
@@ -40786,27 +40786,23 @@
       </c>
       <c r="H179" s="9"/>
       <c r="I179" s="9" t="s">
-        <v>101</v>
+        <v>786</v>
       </c>
       <c r="J179" s="9">
-        <v>16</v>
-      </c>
-      <c r="K179" s="9" t="s">
-        <v>158</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K179" s="9"/>
       <c r="L179" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M179" s="9"/>
       <c r="N179" s="9" t="s">
-        <v>101</v>
+        <v>786</v>
       </c>
       <c r="O179" s="9">
-        <v>16</v>
-      </c>
-      <c r="P179" s="9" t="s">
-        <v>158</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="P179" s="9"/>
       <c r="Q179" s="10"/>
       <c r="R179" s="10"/>
       <c r="S179" s="10"/>
@@ -41160,7 +41156,7 @@
         <v>576</v>
       </c>
       <c r="E181" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F181" s="9"/>
       <c r="G181" s="9" t="s">
@@ -41339,7 +41335,7 @@
         <v>576</v>
       </c>
       <c r="E182" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F182" s="9"/>
       <c r="G182" s="9" t="s">
@@ -41518,7 +41514,7 @@
         <v>576</v>
       </c>
       <c r="E183" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F183" s="9"/>
       <c r="G183" s="9" t="s">
@@ -41697,7 +41693,7 @@
         <v>576</v>
       </c>
       <c r="E184" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F184" s="9"/>
       <c r="G184" s="9" t="s">
@@ -41876,7 +41872,7 @@
         <v>576</v>
       </c>
       <c r="E185" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F185" s="9"/>
       <c r="G185" s="9" t="s">
@@ -42055,7 +42051,7 @@
         <v>576</v>
       </c>
       <c r="E186" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F186" s="9"/>
       <c r="G186" s="9" t="s">
@@ -42234,7 +42230,7 @@
         <v>576</v>
       </c>
       <c r="E187" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F187" s="9"/>
       <c r="G187" s="9" t="s">
@@ -42413,7 +42409,7 @@
         <v>576</v>
       </c>
       <c r="E188" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F188" s="9"/>
       <c r="G188" s="9" t="s">
@@ -42592,7 +42588,7 @@
         <v>576</v>
       </c>
       <c r="E189" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F189" s="9"/>
       <c r="G189" s="9" t="s">
@@ -42950,7 +42946,7 @@
         <v>576</v>
       </c>
       <c r="E191" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F191" s="9"/>
       <c r="G191" s="9" t="s">
@@ -43308,7 +43304,7 @@
         <v>64</v>
       </c>
       <c r="E193" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F193" s="9"/>
       <c r="G193" s="9" t="s">
@@ -55669,7 +55665,7 @@
       </c>
       <c r="J259" s="20">
         <f>SUM(J2:J257)</f>
-        <v>4008</v>
+        <v>3992</v>
       </c>
       <c r="K259" s="20"/>
       <c r="L259" s="34"/>
@@ -55679,7 +55675,7 @@
       </c>
       <c r="O259" s="20">
         <f>SUM(O2:O257)</f>
-        <v>4000</v>
+        <v>3984</v>
       </c>
       <c r="P259" s="34"/>
       <c r="Q259" s="36"/>
@@ -57974,6 +57970,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010075BE519E6FCDE14FB22CB5D8F7193C4B" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a000ce14ad63b1e0207ef1c913f15b8a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="892b2618-d58d-4f46-96dc-04311fd84de8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4a1a096f804483db61bde637f86ae48e" ns2:_="">
     <xsd:import namespace="892b2618-d58d-4f46-96dc-04311fd84de8"/>
@@ -58113,12 +58115,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21877E9D-EFBF-428C-9767-93AD326BBD46}">
   <ds:schemaRefs>
@@ -58128,6 +58124,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89764341-8253-43CB-BA67-8359673E3ECF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="892b2618-d58d-4f46-96dc-04311fd84de8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A169CCE-CE95-4580-B45B-7BEF8291308B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -58143,20 +58155,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89764341-8253-43CB-BA67-8359673E3ECF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="892b2618-d58d-4f46-96dc-04311fd84de8"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>